<commit_message>
Version 2 with station types
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliantecklenborg/VSCode-workspace/GAMI/SALB Benchmark/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliantecklenborg/VSCode-workspace/GAMI/SALB_Benchmark/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732709C4-0775-AD4A-8E8C-8231FD0B880F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F303BFC6-A595-ED46-AC9B-8370CEB06379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2500" yWindow="-17720" windowWidth="28800" windowHeight="15680" xr2:uid="{096A37FF-EAB0-E149-B544-2249525C0269}"/>
+    <workbookView xWindow="-3240" yWindow="-17560" windowWidth="28800" windowHeight="15680" activeTab="4" xr2:uid="{096A37FF-EAB0-E149-B544-2249525C0269}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
     <sheet name="task_times" sheetId="2" r:id="rId2"/>
-    <sheet name="precedence_relations" sheetId="3" r:id="rId3"/>
-    <sheet name="incompatible_tasks" sheetId="4" r:id="rId4"/>
-    <sheet name="compatible_tasks" sheetId="6" r:id="rId5"/>
+    <sheet name="station_types" sheetId="7" r:id="rId3"/>
+    <sheet name="station_costs" sheetId="8" r:id="rId4"/>
+    <sheet name="precedence_relations" sheetId="3" r:id="rId5"/>
+    <sheet name="incompatible_tasks" sheetId="4" r:id="rId6"/>
+    <sheet name="compatible_tasks" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>cycle_time</t>
   </si>
@@ -57,18 +59,12 @@
     <t>task</t>
   </si>
   <si>
-    <t>times_product1</t>
-  </si>
-  <si>
     <t>num_tasks</t>
   </si>
   <si>
     <t>1;2</t>
   </si>
   <si>
-    <t>times_product2</t>
-  </si>
-  <si>
     <t>precedence_relations</t>
   </si>
   <si>
@@ -82,6 +78,30 @@
   </si>
   <si>
     <t>8;9</t>
+  </si>
+  <si>
+    <t>Station_A</t>
+  </si>
+  <si>
+    <t>Station_B</t>
+  </si>
+  <si>
+    <t>Product_A</t>
+  </si>
+  <si>
+    <t>task_ID</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>4;1</t>
+  </si>
+  <si>
+    <t>2;1</t>
   </si>
 </sst>
 </file>
@@ -455,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43D9D4F-CAC2-EB42-8934-6D8C576AA7CA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,12 +505,12 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -503,10 +523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423C713C-314D-7B48-BCE5-A52B358F8186}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,15 +534,118 @@
     <col min="2" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5BA2BE-FFF9-244A-85E1-E8831C5583BC}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -530,10 +653,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -541,10 +664,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -552,10 +675,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -563,10 +686,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -574,10 +697,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -585,10 +708,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -596,10 +719,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -607,10 +730,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -618,10 +741,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -629,10 +752,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -640,12 +763,51 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC8596-6B24-A64E-826E-705EB9729186}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99588B2-D821-AB4E-A83A-1FD5941C0E12}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,12 +817,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -668,12 +840,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88537120-9636-9A43-AD8F-FC1482DA3306}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,12 +855,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -696,7 +868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E06E2C9-810C-D34F-8205-C533EC722C76}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -708,12 +880,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 3 with Gurobi
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliantecklenborg/VSCode-workspace/GAMI/SALB_Benchmark/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F303BFC6-A595-ED46-AC9B-8370CEB06379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79803F16-BD35-7D40-A674-113522A12AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3240" yWindow="-17560" windowWidth="28800" windowHeight="15680" activeTab="4" xr2:uid="{096A37FF-EAB0-E149-B544-2249525C0269}"/>
+    <workbookView xWindow="-720" yWindow="-18560" windowWidth="28800" windowHeight="15680" activeTab="2" xr2:uid="{096A37FF-EAB0-E149-B544-2249525C0269}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
-    <sheet name="task_times" sheetId="2" r:id="rId2"/>
-    <sheet name="station_types" sheetId="7" r:id="rId3"/>
-    <sheet name="station_costs" sheetId="8" r:id="rId4"/>
-    <sheet name="precedence_relations" sheetId="3" r:id="rId5"/>
-    <sheet name="incompatible_tasks" sheetId="4" r:id="rId6"/>
-    <sheet name="compatible_tasks" sheetId="6" r:id="rId7"/>
+    <sheet name="cycle_time" sheetId="10" r:id="rId2"/>
+    <sheet name="task_times" sheetId="2" r:id="rId3"/>
+    <sheet name="station_types" sheetId="7" r:id="rId4"/>
+    <sheet name="station_costs" sheetId="8" r:id="rId5"/>
+    <sheet name="precedence_relations" sheetId="3" r:id="rId6"/>
+    <sheet name="incompatible_tasks" sheetId="4" r:id="rId7"/>
+    <sheet name="compatible_tasks" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,10 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
-  <si>
-    <t>cycle_time</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>num_products</t>
   </si>
@@ -71,24 +69,9 @@
     <t>incompatible_tasks</t>
   </si>
   <si>
-    <t>6;7</t>
-  </si>
-  <si>
     <t>compatible_tasks</t>
   </si>
   <si>
-    <t>8;9</t>
-  </si>
-  <si>
-    <t>Station_A</t>
-  </si>
-  <si>
-    <t>Station_B</t>
-  </si>
-  <si>
-    <t>Product_A</t>
-  </si>
-  <si>
     <t>task_ID</t>
   </si>
   <si>
@@ -98,20 +81,155 @@
     <t>Costs</t>
   </si>
   <si>
-    <t>4;1</t>
-  </si>
-  <si>
-    <t>2;1</t>
+    <t>TXP-M2/K2</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>2;3</t>
+  </si>
+  <si>
+    <t>3;4</t>
+  </si>
+  <si>
+    <t>4;5</t>
+  </si>
+  <si>
+    <t>5;9</t>
+  </si>
+  <si>
+    <t>9;10</t>
+  </si>
+  <si>
+    <t>10;12</t>
+  </si>
+  <si>
+    <t>12;14</t>
+  </si>
+  <si>
+    <t>14;16</t>
+  </si>
+  <si>
+    <t>16;23</t>
+  </si>
+  <si>
+    <t>23;28</t>
+  </si>
+  <si>
+    <t>28;31</t>
+  </si>
+  <si>
+    <t>31;34</t>
+  </si>
+  <si>
+    <t>34;36</t>
+  </si>
+  <si>
+    <t>36;40</t>
+  </si>
+  <si>
+    <t>40;49</t>
+  </si>
+  <si>
+    <t>49;52</t>
+  </si>
+  <si>
+    <t>52;54</t>
+  </si>
+  <si>
+    <t>54;57</t>
+  </si>
+  <si>
+    <t>57;60</t>
+  </si>
+  <si>
+    <t>60;63</t>
+  </si>
+  <si>
+    <t>63;67</t>
+  </si>
+  <si>
+    <t>67;71</t>
+  </si>
+  <si>
+    <t>71;75</t>
+  </si>
+  <si>
+    <t>75;77</t>
+  </si>
+  <si>
+    <t>77;80</t>
+  </si>
+  <si>
+    <t>80;83</t>
+  </si>
+  <si>
+    <t>83;86</t>
+  </si>
+  <si>
+    <t>86;87</t>
+  </si>
+  <si>
+    <t>87;88</t>
+  </si>
+  <si>
+    <t>88;90</t>
+  </si>
+  <si>
+    <t>90;93</t>
+  </si>
+  <si>
+    <t>93;96</t>
+  </si>
+  <si>
+    <t>96;98</t>
+  </si>
+  <si>
+    <t>98;99</t>
+  </si>
+  <si>
+    <t>99;101</t>
+  </si>
+  <si>
+    <t>101;103</t>
+  </si>
+  <si>
+    <t>103;104</t>
+  </si>
+  <si>
+    <t>11;12</t>
+  </si>
+  <si>
+    <t>10;11</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Cycle_time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -473,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43D9D4F-CAC2-EB42-8934-6D8C576AA7CA}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,10 +604,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -497,23 +615,15 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -522,11 +632,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A9D7FC-5863-4C4C-B771-6FE379A8C4FC}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423C713C-314D-7B48-BCE5-A52B358F8186}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,92 +683,455 @@
     <col min="2" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>34</v>
+      </c>
+      <c r="B16">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>52</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>54</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>57</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>60</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>63</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>67</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>71</v>
+      </c>
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>75</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>77</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>80</v>
+      </c>
+      <c r="B29">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="C29">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>83</v>
+      </c>
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>86</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>87</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>88</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>90</v>
+      </c>
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>93</v>
+      </c>
+      <c r="B35">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>96</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>98</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>99</v>
+      </c>
+      <c r="B38">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>101</v>
+      </c>
+      <c r="B39">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>6</v>
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>103</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>104</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -627,25 +1139,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5BA2BE-FFF9-244A-85E1-E8831C5583BC}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -697,7 +1209,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -705,10 +1217,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -716,21 +1228,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -738,23 +1250,353 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>52</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>54</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>57</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>60</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>63</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>67</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>71</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>75</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>77</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>80</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>83</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>86</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>87</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>88</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>90</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>93</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>96</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>98</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>99</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>101</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>103</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>104</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
         <v>1</v>
       </c>
     </row>
@@ -763,38 +1605,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AC8596-6B24-A64E-826E-705EB9729186}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>50000</v>
       </c>
     </row>
   </sheetData>
@@ -802,12 +1644,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99588B2-D821-AB4E-A83A-1FD5941C0E12}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,36 +1659,220 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88537120-9636-9A43-AD8F-FC1482DA3306}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -855,12 +1881,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -868,24 +1889,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E06E2C9-810C-D34F-8205-C533EC722C76}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>